<commit_message>
Update spreadsheets intro section
</commit_message>
<xml_diff>
--- a/0_Resources/Problems/1_Spreadsheets_Intro/1_Spreadsheets_Intro_Solution.xlsx
+++ b/0_Resources/Problems/1_Spreadsheets_Intro/1_Spreadsheets_Intro_Solution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\0_Resources\Problems\1_Spreadsheets_Intro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D8EB6E-780A-4A54-A0DC-19098264667D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23AA10E-8E3C-4B20-9601-E1783ABD291D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="18330" windowHeight="12855" activeTab="1" xr2:uid="{86D7107E-0634-4B38-BA6C-8A80968FF286}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{86D7107E-0634-4B38-BA6C-8A80968FF286}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Worksheets" sheetId="1" r:id="rId1"/>
@@ -660,7 +660,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>